<commit_message>
Update as of 11/12/2019
</commit_message>
<xml_diff>
--- a/ANALYSIS/Isolated Limb Movements/Limb_Movements_Offline/CleanEEGwithICA.xlsx
+++ b/ANALYSIS/Isolated Limb Movements/Limb_Movements_Offline/CleanEEGwithICA.xlsx
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2267,5 +2267,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>